<commit_message>
Fix: deleted obsolete docu
</commit_message>
<xml_diff>
--- a/testdata/user-mapping-template.example.xlsx
+++ b/testdata/user-mapping-template.example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flake/sources/misc/secman/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBE7F7E-1BDC-5F41-A4C7-8F736E039C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0840AF42-7295-8847-9ABF-DE4CDDC7F3B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="21660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -195,12 +195,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -507,13 +509,13 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="2" max="2" width="18" style="6" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
   </cols>
   <sheetData>
@@ -521,7 +523,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -532,7 +534,7 @@
       <c r="A2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="6">
         <v>199619961996</v>
       </c>
       <c r="C2" t="s">
@@ -543,7 +545,7 @@
       <c r="A3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>35</v>
       </c>
       <c r="C3" t="s">
@@ -554,7 +556,7 @@
       <c r="A4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="6">
         <v>199719971997</v>
       </c>
       <c r="C4" t="s">

</xml_diff>